<commit_message>
creating custom halloween html
</commit_message>
<xml_diff>
--- a/exampleSite/static/halloween_costume_generator.xlsx
+++ b/exampleSite/static/halloween_costume_generator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hugo\Sites\robinzng\exampleSite\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A26EE5-758F-4D58-93A9-783612C1958A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1D3263-A23D-4C47-9677-BE977C472F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{43372864-43D7-4A59-ACF3-6134C87F189E}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="92">
   <si>
     <t>character</t>
   </si>
@@ -177,9 +177,6 @@
     <t>Daria Morgendorffer</t>
   </si>
   <si>
-    <t>brown hair, round glasses</t>
-  </si>
-  <si>
     <t>green blazer, green jacket, orange shirt, orange top, orange blouse</t>
   </si>
   <si>
@@ -198,13 +195,124 @@
     <t>red blazer, red jacket, black shirt, black blouse, black v-neck</t>
   </si>
   <si>
-    <t>black hair, black bob, earrings</t>
-  </si>
-  <si>
     <t>grey shorts, black shorts</t>
   </si>
   <si>
     <t>black tights, black boots, black knee-high boots</t>
+  </si>
+  <si>
+    <t>Quinn Morgendorffer</t>
+  </si>
+  <si>
+    <t>https://th.bing.com/th/id/R.e65c73bba6f6ae5d6f882f7932ce2d4c?rik=7UN34tNBhRF77g&amp;riu=http%3a%2f%2fimg2.wikia.nocookie.net%2f__cb20130604070322%2fdaria%2fimages%2f8%2f8b%2fImg-thing.jpg&amp;ehk=Df7ytuLZKvLFc%2bfDnDQdfQCoNrc%2f%2btcAowq7t5B2UtE%3d&amp;risl=&amp;pid=ImgRaw&amp;r=0</t>
+  </si>
+  <si>
+    <t>red hair, bangs, redhead</t>
+  </si>
+  <si>
+    <t>pink shirt, smiley face tee</t>
+  </si>
+  <si>
+    <t>black boots, black shoes</t>
+  </si>
+  <si>
+    <t>Trent Lane</t>
+  </si>
+  <si>
+    <t>https://static.wikia.nocookie.net/daria/images/f/f3/Trentcropped.png/revision/latest?cb=20200815062032</t>
+  </si>
+  <si>
+    <t>accessories</t>
+  </si>
+  <si>
+    <t>green shirt, green tee</t>
+  </si>
+  <si>
+    <t>spiky black hair, goatee</t>
+  </si>
+  <si>
+    <t>necklace, cuff bracelet, rings, earrings</t>
+  </si>
+  <si>
+    <t>brown belt</t>
+  </si>
+  <si>
+    <t>black hair, black bob</t>
+  </si>
+  <si>
+    <t>earrings</t>
+  </si>
+  <si>
+    <t>brown hair</t>
+  </si>
+  <si>
+    <t>round glasses</t>
+  </si>
+  <si>
+    <t>Brittany Taylor</t>
+  </si>
+  <si>
+    <t>https://static.miraheze.org/dariawikiwiki/c/c5/Brittany.gif</t>
+  </si>
+  <si>
+    <t>blonde pigtails, blond hair</t>
+  </si>
+  <si>
+    <t>blue shirt</t>
+  </si>
+  <si>
+    <t>yellow skirt, blue skirt, pleated skirt</t>
+  </si>
+  <si>
+    <t>pom-poms</t>
+  </si>
+  <si>
+    <t>yellow socks, blue sneakers, blue shoes</t>
+  </si>
+  <si>
+    <t>Kevin Thompson</t>
+  </si>
+  <si>
+    <t>black hair</t>
+  </si>
+  <si>
+    <t>yellow football jersey, yellow shirt</t>
+  </si>
+  <si>
+    <t>blue pants, jeans, blue leggings</t>
+  </si>
+  <si>
+    <t>flare jeans, blue jeans, flared pants, blue pants</t>
+  </si>
+  <si>
+    <t>neck cushion, football equipment, gloves</t>
+  </si>
+  <si>
+    <t>cleats, white sneakers</t>
+  </si>
+  <si>
+    <t>Jodie Landon</t>
+  </si>
+  <si>
+    <t>https://th.bing.com/th/id/R.58bd988ef1a6fdb387eb2c760efc707f?rik=qbnGZ8NksR7AjA&amp;riu=http%3a%2f%2fvignette4.wikia.nocookie.net%2fdaria%2fimages%2f1%2f14%2fKevin_Thompson.gif%2frevision%2flatest%3fcb%3d20140902121519&amp;ehk=zzgrLHBjr0sgpwmYGZ%2fVDP43hK2tTkgKGckfZC7drhc%3d&amp;risl=&amp;pid=ImgRaw&amp;r=0</t>
+  </si>
+  <si>
+    <t>black hair, black braids</t>
+  </si>
+  <si>
+    <t>pink shirt, pink blouse</t>
+  </si>
+  <si>
+    <t>grey skirt, white skirt, miniskirt</t>
+  </si>
+  <si>
+    <t>books</t>
+  </si>
+  <si>
+    <t>black shoes, black mary janes, black loafers</t>
+  </si>
+  <si>
+    <t>https://static.tvtropes.org/pmwiki/pub/images/jodie_8099.gif</t>
   </si>
 </sst>
 </file>
@@ -559,18 +667,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD77BA2C-ED9F-412B-B177-4CBE1A214489}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="8" width="9.7265625" customWidth="1"/>
+    <col min="1" max="9" width="9.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
@@ -593,10 +701,13 @@
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -607,39 +718,169 @@
         <v>43</v>
       </c>
       <c r="D2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" t="s">
         <v>46</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>47</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" t="s">
         <v>48</v>
       </c>
-      <c r="H2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>44</v>
       </c>
       <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
         <v>50</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" t="s">
         <v>51</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" t="s">
+        <v>67</v>
+      </c>
+      <c r="I3" t="s">
         <v>53</v>
       </c>
-      <c r="E3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" t="s">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
         <v>54</v>
       </c>
-      <c r="H3" t="s">
+      <c r="C4" t="s">
         <v>55</v>
+      </c>
+      <c r="D4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" t="s">
+        <v>74</v>
+      </c>
+      <c r="H6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" t="s">
+        <v>80</v>
+      </c>
+      <c r="H7" t="s">
+        <v>82</v>
+      </c>
+      <c r="I7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F8" t="s">
+        <v>88</v>
+      </c>
+      <c r="H8" t="s">
+        <v>89</v>
+      </c>
+      <c r="I8" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>